<commit_message>
Added a data.gov get test method
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData.xlsx
+++ b/src/test/resources/ExcelTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/Documents/workspace-sts-3.8.3.RELEASE/rest-assured-docker/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/Documents/workspace-sts-3.8.3.RELEASE/rest-assured-simpler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/api/3/action/help_show?name=package_search</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>TestCase_003</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/api/3/action/package_search</t>
   </si>
 </sst>
 </file>
@@ -404,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,10 +480,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added other nasa and gov domain services
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData.xlsx
+++ b/src/test/resources/ExcelTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -81,6 +81,30 @@
   </si>
   <si>
     <t>https://catalog.data.gov/api/3/action/package_search</t>
+  </si>
+  <si>
+    <t>https://api.nasa.gov/planetary/apod?api_key=NNKOjkoul8n1CH18TWA9gwngW1s1SmjESPjNoUFo</t>
+  </si>
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>TestCase_004</t>
+  </si>
+  <si>
+    <t>https://api.nasa.gov/mars-photos/api/v1/rovers/curiosity/photos?sol=1000&amp;page=2&amp;api_key=DEMO_KEY</t>
+  </si>
+  <si>
+    <t>photos[1].rover.name</t>
+  </si>
+  <si>
+    <t>Curiosity</t>
+  </si>
+  <si>
+    <t>TestCase_005</t>
   </si>
 </sst>
 </file>
@@ -416,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,6 +521,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
Replacing image with video
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData.xlsx
+++ b/src/test/resources/ExcelTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/Documents/workspace-sts-3.8.3.RELEASE/rest-assured-simpler/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/code/githubws/rest-assured-simpler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -89,9 +89,6 @@
     <t>media_type</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>TestCase_004</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>TestCase_005</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +523,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -532,7 +532,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
@@ -540,16 +540,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Removed 1 failing test data
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData.xlsx
+++ b/src/test/resources/ExcelTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/code/githubws/rest-assured-simpler/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/code/gitws/rest-assured-simpler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -90,18 +90,6 @@
   </si>
   <si>
     <t>TestCase_004</t>
-  </si>
-  <si>
-    <t>https://api.nasa.gov/mars-photos/api/v1/rovers/curiosity/photos?sol=1000&amp;page=2&amp;api_key=DEMO_KEY</t>
-  </si>
-  <si>
-    <t>photos[1].rover.name</t>
-  </si>
-  <si>
-    <t>Curiosity</t>
-  </si>
-  <si>
-    <t>TestCase_005</t>
   </si>
   <si>
     <t>video</t>
@@ -440,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,26 +520,9 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed data for all 5
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData.xlsx
+++ b/src/test/resources/ExcelTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/code/gitws/rest-assured-simpler/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -92,7 +92,19 @@
     <t>TestCase_004</t>
   </si>
   <si>
-    <t>video</t>
+    <t>https://api.nasa.gov/mars-photos/api/v1/rovers/curiosity/photos?sol=1000&amp;page=2&amp;api_key=DEMO_KEY</t>
+  </si>
+  <si>
+    <t>photos[1].rover.name</t>
+  </si>
+  <si>
+    <t>Curiosity</t>
+  </si>
+  <si>
+    <t>TestCase_005</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -428,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,9 +532,26 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed all data.gov and nasa data
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData.xlsx
+++ b/src/test/resources/ExcelTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityai/code/gitws/rest-assured-simpler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -440,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,6 +505,81 @@
         <v>12</v>
       </c>
     </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>

</xml_diff>